<commit_message>
started on Leg lookup table
</commit_message>
<xml_diff>
--- a/OrLawsLookup.xlsx
+++ b/OrLawsLookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\leg\lc\home\MaugerR\mORS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobby\mORS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55758BD2-64AD-415F-9139-DF862944C4FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D5AB68-6EC5-4657-832D-48FC9228B217}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="1590" windowWidth="11820" windowHeight="18525" xr2:uid="{FD0EEE08-64EB-4AD4-AC40-D23941B49031}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="9420" xr2:uid="{FD0EEE08-64EB-4AD4-AC40-D23941B49031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>pdfs:</t>
-  </si>
-  <si>
-    <t>2013, 2015-2021</t>
+    <t>bills_laws/lawsstatutes/2014R1orLaw$$$$ss.pdf</t>
   </si>
 </sst>
 </file>
@@ -390,25 +387,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88258278-46C6-4AF8-B1A1-B9F85335FFB8}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2013</v>
+      </c>
+      <c r="B1" t="str">
+        <f t="shared" ref="B1:B7" si="0">"bills_laws/lawsstatutes/"&amp;A1&amp;"orlaw$$$$.pdf"</f>
+        <v>bills_laws/lawsstatutes/2013orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2015orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2016orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2017orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2018orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2019orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2020</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>bills_laws/lawsstatutes/2020orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2021</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"bills_laws/lawsstatutes/"&amp;A8&amp;"orlaw$$$$.pdf"</f>
+        <v>bills_laws/lawsstatutes/2021orlaw$$$$.pdf</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2014</v>
+      </c>
+      <c r="B9" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>2014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>